<commit_message>
feat: Create test FCs for CRS proiling
</commit_message>
<xml_diff>
--- a/fc_profiler_tests.xlsx
+++ b/fc_profiler_tests.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="54" documentId="11_CA44E1CCD3E4EB3E99BCD189F8C4523140F1EFCE" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{AE0CCAB1-B40E-4FD4-BBBD-5D0C926EBAF6}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="11_CA44E1CCD3E4EB3E99BCD189F8C4523140F1EFCE" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{35FDAA4D-EC51-4DDC-ABBA-E1D68AEFB71A}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tests" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="54">
   <si>
     <t>function</t>
   </si>
@@ -109,57 +109,15 @@
     <t>nonexistant.gdb\nonexistant_fc</t>
   </si>
   <si>
-    <t>test.gdb\nonexistant_fc</t>
-  </si>
-  <si>
-    <t>test.gdb\test_fc</t>
-  </si>
-  <si>
     <t>long_folder_name_&lt;260_chars&gt;\test.gdb\test_fc</t>
   </si>
   <si>
-    <t>tyest.gdb\zero_rows_fc</t>
-  </si>
-  <si>
-    <t>test.gdb\four_million_rows_fc</t>
-  </si>
-  <si>
-    <t>test.gdb\has_z_values_fc</t>
-  </si>
-  <si>
-    <t>test.gdb\has_no_z_values_fc</t>
-  </si>
-  <si>
-    <t>test.gdb\has_m_values_fc</t>
-  </si>
-  <si>
-    <t>test.gdb\has_m_z_values_fc</t>
-  </si>
-  <si>
-    <t>test.gdb\GDA_LL_point</t>
-  </si>
-  <si>
-    <t>test.gdb\WGS84_LL_point</t>
-  </si>
-  <si>
-    <t>test.gdb\MGAZ55_point</t>
-  </si>
-  <si>
-    <t>test.gdb\GDA94_GA_Lambert_point</t>
-  </si>
-  <si>
-    <t>test.gdb\Web_Mercator_point</t>
-  </si>
-  <si>
     <t>units=degrees</t>
   </si>
   <si>
     <t>units= meters</t>
   </si>
   <si>
-    <t>test.gdb\no_projection</t>
-  </si>
-  <si>
     <t>CRS=WGS84 Lat Long</t>
   </si>
   <si>
@@ -176,6 +134,54 @@
   </si>
   <si>
     <t>CRS=none</t>
+  </si>
+  <si>
+    <t>input_fgdb</t>
+  </si>
+  <si>
+    <t>test.gdb</t>
+  </si>
+  <si>
+    <t>GDA_LL_point</t>
+  </si>
+  <si>
+    <t>WGS84_LL_point</t>
+  </si>
+  <si>
+    <t>Web_Mercator_point</t>
+  </si>
+  <si>
+    <t>MGAZ55_point</t>
+  </si>
+  <si>
+    <t>GDA94_GA_Lambert_point</t>
+  </si>
+  <si>
+    <t>nonexistant_fc</t>
+  </si>
+  <si>
+    <t>zero_rows_fc</t>
+  </si>
+  <si>
+    <t>four_million_rows_fc</t>
+  </si>
+  <si>
+    <t>has_z_values_fc</t>
+  </si>
+  <si>
+    <t>has_no_z_values_fc</t>
+  </si>
+  <si>
+    <t>has_m_values_fc</t>
+  </si>
+  <si>
+    <t>has_m_z_values_fc</t>
+  </si>
+  <si>
+    <t>NO_CRS_point</t>
+  </si>
+  <si>
+    <t>meters</t>
   </si>
 </sst>
 </file>
@@ -503,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,11 +521,12 @@
     <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" customWidth="1"/>
     <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="52.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,127 +540,146 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="E7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
@@ -664,58 +690,67 @@
         <v>11</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="1"/>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -723,129 +758,185 @@
       <c r="D14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="2"/>
+      <c r="F14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
         <v>5</v>
       </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
         <v>7</v>
       </c>
-      <c r="E15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="E16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19">
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20">
         <v>4000000</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="E20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>21</v>
+      <c r="C22" t="s">
+        <v>11</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>37</v>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>